<commit_message>
EO sensor calculations are working
</commit_message>
<xml_diff>
--- a/UAV/SensorCalculations.xlsx
+++ b/UAV/SensorCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\repo\uav-sysml\UAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016720B0-6A6C-4549-81D8-CC44D775A2E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACDCF1-359C-45A0-BB3A-A544184479C5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="23025" xr2:uid="{2D98E863-B19C-4883-B20A-28903A85B63A}"/>
   </bookViews>
@@ -19,18 +19,20 @@
     <definedName name="CruisingVelocity">Sheet1!$C$17</definedName>
     <definedName name="Dc_Human">Sheet1!$C$5</definedName>
     <definedName name="Dc_Vehicle">Sheet1!$C$6</definedName>
-    <definedName name="EO_Ground_Coverage_Rate">Sheet1!$G$11</definedName>
-    <definedName name="EO_GroundSwath">Sheet1!$G$10</definedName>
-    <definedName name="EO_N_Human">Sheet1!$G$7</definedName>
-    <definedName name="EO_N_Vehicle">Sheet1!$G$8</definedName>
+    <definedName name="EO_Ground_Coverage_Rate">Sheet1!$F$11</definedName>
+    <definedName name="EO_GroundSwath">Sheet1!$F$10</definedName>
+    <definedName name="EO_N_Human">Sheet1!$F$7</definedName>
+    <definedName name="EO_N_Vehicle">Sheet1!$F$8</definedName>
     <definedName name="EOFOV">Sheet1!$C$13</definedName>
-    <definedName name="EOGSDh">Sheet1!$G$4</definedName>
-    <definedName name="EOGSDv">Sheet1!$G$5</definedName>
+    <definedName name="EOGSDh">Sheet1!$F$4</definedName>
+    <definedName name="EOGSDv">Sheet1!$F$5</definedName>
     <definedName name="EOHoriz">Sheet1!$C$14</definedName>
     <definedName name="EOVert">Sheet1!$C$15</definedName>
     <definedName name="FeetToMeters">Sheet1!$C$3</definedName>
     <definedName name="OperatingAltitude">Sheet1!$C$16</definedName>
-    <definedName name="Prob_Day_Human">Sheet1!$G$13</definedName>
+    <definedName name="Prob_Day_Human">Sheet1!$F$13</definedName>
+    <definedName name="Prob_Day_Vehicle">Sheet1!$F$15</definedName>
+    <definedName name="T_Scan_5km_Box">Sheet1!$F$17</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>EO GSDh</t>
   </si>
@@ -105,14 +107,34 @@
   </si>
   <si>
     <t>Denominator</t>
+  </si>
+  <si>
+    <t>Probability of Detecting a Vehicle in the Daytime</t>
+  </si>
+  <si>
+    <t>Time to scan a 5km by 5km box during the daytime</t>
+  </si>
+  <si>
+    <t>IR Calculations</t>
+  </si>
+  <si>
+    <t>IR FOV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,8 +162,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,28 +479,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC759366-37BF-4214-B2FC-359392225ECA}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -486,22 +512,22 @@
         <v>0.30478512648582745</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>0.75</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <f>2 * TAN((EOFOV * PI() / 180) / (2 * EOHoriz)) * OperatingAltitude * FeetToMeters</f>
         <v>0.7979260509843894</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -509,15 +535,15 @@
         <f>SQRT(0.5 *1.75)</f>
         <v>0.93541434669348533</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <f>2 * TAN((EOFOV * PI() / 180) / (2 * EOVert)) * OperatingAltitude * FeetToMeters</f>
         <v>0.7979260509843894</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -526,109 +552,146 @@
         <v>5.387374128459987</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <f>Dc_Human/(EOGSDh+EOGSDv)</f>
         <v>0.58615353236022227</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <f>Dc_Vehicle/(EOGSDh+EOGSDv)</f>
         <v>3.3758605335755516</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <f>(TAN(0.5 *EOFOV*PI()/180)-TAN(-0.5*EOFOV*PI()/180))*OperatingAltitude/3.281</f>
         <v>163.33385701379012</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <f>EO_GroundSwath*CruisingVelocity*1.852/3.6</f>
         <v>8402.6195330427599</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13">
         <v>30</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="G13">
-        <f>J13/J14</f>
+      <c r="F13">
+        <f>I13/I14</f>
         <v>0.30994496004949795</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" t="s">
         <v>19</v>
       </c>
-      <c r="J13">
+      <c r="I13">
         <f>(EO_N_Human/0.75)^(2.7+0.7*(EO_N_Human/C4))</f>
         <v>0.44915976567859056</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14">
         <v>200</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" t="s">
         <v>20</v>
       </c>
-      <c r="J14">
+      <c r="I14">
         <f>1+(EO_N_Human/0.75)^(2.7+0.7*(EO_N_Human/C4))</f>
         <v>1.4491597656785906</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15">
         <v>200</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <f>I15/I16</f>
+        <v>0.99117719383448366</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <f>(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C6))</f>
+        <v>112.34262379110956</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16">
         <v>1000</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <f>1+(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C6))</f>
+        <v>113.34262379110956</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <f>25000000*60/EO_Ground_Coverage_Rate</f>
+        <v>178515.75857996981</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP, non-working after adding IR calculations
</commit_message>
<xml_diff>
--- a/UAV/SensorCalculations.xlsx
+++ b/UAV/SensorCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\repo\uav-sysml\UAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACDCF1-359C-45A0-BB3A-A544184479C5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF10CEBB-DF0F-4779-BB5E-E5713AD8F584}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="23025" xr2:uid="{2D98E863-B19C-4883-B20A-28903A85B63A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CruisingVelocity">Sheet1!$C$17</definedName>
+    <definedName name="CruisingVelocity">Sheet1!$C$18</definedName>
     <definedName name="Dc_Human">Sheet1!$C$5</definedName>
     <definedName name="Dc_Vehicle">Sheet1!$C$6</definedName>
     <definedName name="EO_Ground_Coverage_Rate">Sheet1!$F$11</definedName>
@@ -29,10 +29,23 @@
     <definedName name="EOHoriz">Sheet1!$C$14</definedName>
     <definedName name="EOVert">Sheet1!$C$15</definedName>
     <definedName name="FeetToMeters">Sheet1!$C$3</definedName>
-    <definedName name="OperatingAltitude">Sheet1!$C$16</definedName>
+    <definedName name="IR_Ground_Coverage_Rate">Sheet1!$F$27</definedName>
+    <definedName name="IR_GroundSwath">Sheet1!$F$26</definedName>
+    <definedName name="IR_N_Human">Sheet1!$F$23</definedName>
+    <definedName name="IR_N_Vehicle">Sheet1!$F$24</definedName>
+    <definedName name="IRFOV">Sheet1!$C$20</definedName>
+    <definedName name="IRGSDh">Sheet1!$F$20</definedName>
+    <definedName name="IRGSDv">Sheet1!$F$21</definedName>
+    <definedName name="IRHoriz">Sheet1!$C$21</definedName>
+    <definedName name="IRVert">Sheet1!$C$22</definedName>
+    <definedName name="OperatingAltitude">Sheet1!$C$17</definedName>
     <definedName name="Prob_Day_Human">Sheet1!$F$13</definedName>
     <definedName name="Prob_Day_Vehicle">Sheet1!$F$15</definedName>
+    <definedName name="Prob_Night_Human">Sheet1!$F$29</definedName>
+    <definedName name="Prob_Night_Vehicle">Sheet1!$F$31</definedName>
     <definedName name="T_Scan_5km_Box">Sheet1!$F$17</definedName>
+    <definedName name="T_Scan_5km_Box_Day">Sheet1!$F$17</definedName>
+    <definedName name="T_Scan_5km_Box_Night">Sheet1!$F$33</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -44,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>EO GSDh</t>
   </si>
@@ -119,6 +132,39 @@
   </si>
   <si>
     <t>IR FOV</t>
+  </si>
+  <si>
+    <t>IR Horizontal</t>
+  </si>
+  <si>
+    <t>IR Vertical</t>
+  </si>
+  <si>
+    <t>IR GSDh</t>
+  </si>
+  <si>
+    <t>IR GSDv</t>
+  </si>
+  <si>
+    <t>IR_N_Human</t>
+  </si>
+  <si>
+    <t>IR_N_Vehicle</t>
+  </si>
+  <si>
+    <t>IR_GroundSwath</t>
+  </si>
+  <si>
+    <t>IR_Ground_Coverage_Rate</t>
+  </si>
+  <si>
+    <t>Probability of Detecting a Human at Night</t>
+  </si>
+  <si>
+    <t>Probability of Detecting a Vehicle at Night</t>
+  </si>
+  <si>
+    <t>Time to scan a 5km by 5km box at Night</t>
   </si>
 </sst>
 </file>
@@ -479,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC759366-37BF-4214-B2FC-359392225ECA}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +672,7 @@
         <v>20</v>
       </c>
       <c r="I14">
-        <f>1+(EO_N_Human/0.75)^(2.7+0.7*(EO_N_Human/C4))</f>
+        <f>1+I13</f>
         <v>1.4491597656785906</v>
       </c>
     </row>
@@ -642,37 +688,31 @@
       </c>
       <c r="F15">
         <f>I15/I16</f>
-        <v>0.99117719383448366</v>
+        <v>0.99984952338788302</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15">
-        <f>(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C6))</f>
-        <v>112.34262379110956</v>
+        <f>(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C4))</f>
+        <v>6644.5509991328045</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>1000</v>
-      </c>
       <c r="H16" t="s">
         <v>20</v>
       </c>
       <c r="I16">
-        <f>1+(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C6))</f>
-        <v>113.34262379110956</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <f>1+I15</f>
+        <v>6645.5509991328045</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="E17" t="s">
         <v>22</v>
@@ -682,12 +722,150 @@
         <v>178515.75857996981</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <f>2*TAN((IRFOV*PI()/180)/(2*IRHoriz))*OperatingAltitude*FeetToMeters</f>
+        <v>1.1968899309934578</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21">
+        <f>2*TAN((IRFOV*PI()/180)/(2*IRVert))*OperatingAltitude*FeetToMeters</f>
+        <v>1.1968899309934578</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <f>Dc_Human/(IRGSDh+IRGSDv)</f>
+        <v>0.39076874258481764</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <f>Dc_Vehicle/(IRGSDh+IRGSDv)</f>
+        <v>2.2505720822583455</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <f>(TAN(0.5*IRFOV*PI()/180)-TAN(-0.5*IRFOV*PI()/180))*OperatingAltitude/3.281</f>
+        <v>252.49226600005792</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27">
+        <f>IR_GroundSwath*CruisingVelocity*1.852/3.6</f>
+        <v>12989.324350891871</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29">
+        <f>I29/I30</f>
+        <v>0.11940624924274684</v>
+      </c>
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29">
+        <f>(IR_N_Human/0.75)^(2.7+0.7*(IR_N_Human/C4))</f>
+        <v>0.13559742973427333</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30">
+        <f>1+I29</f>
+        <v>1.1355974297342732</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31">
+        <f>I31/I32</f>
+        <v>0.99490884300249272</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31">
+        <f>(IR_N_Vehicle/0.75)^(2.7+0.7*(IR_N_Vehicle/C4))</f>
+        <v>195.41900662062224</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <f>1+I31</f>
+        <v>196.41900662062224</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33">
+        <f>25000000*60/IR_Ground_Coverage_Rate</f>
+        <v>115479.44754316703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Order-of-magnitude correction for 'time to scan' calculations. Divide by 1000.
</commit_message>
<xml_diff>
--- a/UAV/SensorCalculations.xlsx
+++ b/UAV/SensorCalculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\repo\uav-sysml\UAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF10CEBB-DF0F-4779-BB5E-E5713AD8F584}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01EA2F2-828B-4585-8D85-C87DACB8431D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48000" windowHeight="23025" xr2:uid="{2D98E863-B19C-4883-B20A-28903A85B63A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18450" windowHeight="11475" xr2:uid="{2D98E863-B19C-4883-B20A-28903A85B63A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,7 +528,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="F4">
         <f>2 * TAN((EOFOV * PI() / 180) / (2 * EOHoriz)) * OperatingAltitude * FeetToMeters</f>
-        <v>0.7979260509843894</v>
+        <v>0.17731680394411209</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
       </c>
       <c r="F5">
         <f>2 * TAN((EOFOV * PI() / 180) / (2 * EOVert)) * OperatingAltitude * FeetToMeters</f>
-        <v>0.7979260509843894</v>
+        <v>0.17731680394411209</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
       </c>
       <c r="F7">
         <f>Dc_Human/(EOGSDh+EOGSDv)</f>
-        <v>0.58615353236022227</v>
+        <v>2.6376923277624482</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
       </c>
       <c r="F8">
         <f>Dc_Vehicle/(EOGSDh+EOGSDv)</f>
-        <v>3.3758605335755516</v>
+        <v>15.191380649286957</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
       </c>
       <c r="F10">
         <f>(TAN(0.5 *EOFOV*PI()/180)-TAN(-0.5*EOFOV*PI()/180))*OperatingAltitude/3.281</f>
-        <v>163.33385701379012</v>
+        <v>351.9355496431732</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
       </c>
       <c r="F11">
         <f>EO_GroundSwath*CruisingVelocity*1.852/3.6</f>
-        <v>8402.6195330427599</v>
+        <v>18105.128831643244</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -644,21 +644,21 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13">
         <f>I13/I14</f>
-        <v>0.30994496004949795</v>
+        <v>0.99848597434398856</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="I13">
         <f>(EO_N_Human/0.75)^(2.7+0.7*(EO_N_Human/C4))</f>
-        <v>0.44915976567859056</v>
+        <v>659.49078893049568</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -666,14 +666,14 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <v>200</v>
+        <v>1800</v>
       </c>
       <c r="H14" t="s">
         <v>20</v>
       </c>
       <c r="I14">
         <f>1+I13</f>
-        <v>1.4491597656785906</v>
+        <v>660.49078893049568</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -681,21 +681,21 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>200</v>
+        <v>1800</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
       </c>
       <c r="F15">
         <f>I15/I16</f>
-        <v>0.99984952338788302</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15">
         <f>(EO_N_Vehicle/0.75)^(2.7+0.7*(EO_N_Vehicle/C4))</f>
-        <v>6644.5509991328045</v>
+        <v>1.1285658378597852E+22</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
       </c>
       <c r="I16">
         <f>1+I15</f>
-        <v>6645.5509991328045</v>
+        <v>1.1285658378597852E+22</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -718,8 +718,8 @@
         <v>22</v>
       </c>
       <c r="F17">
-        <f>25000000*60/EO_Ground_Coverage_Rate</f>
-        <v>178515.75857996981</v>
+        <f>25000*60/EO_Ground_Coverage_Rate</f>
+        <v>82.849451884505484</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -740,14 +740,14 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20">
         <f>2*TAN((IRFOV*PI()/180)/(2*IRHoriz))*OperatingAltitude*FeetToMeters</f>
-        <v>1.1968899309934578</v>
+        <v>0.39896285458905412</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -755,14 +755,14 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
       </c>
       <c r="F21">
         <f>2*TAN((IRFOV*PI()/180)/(2*IRVert))*OperatingAltitude*FeetToMeters</f>
-        <v>1.1968899309934578</v>
+        <v>0.39896285458905412</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>200</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
       </c>
       <c r="F23">
         <f>Dc_Human/(IRGSDh+IRGSDv)</f>
-        <v>0.39076874258481764</v>
+        <v>1.1723075668999252</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
       </c>
       <c r="F24">
         <f>Dc_Vehicle/(IRGSDh+IRGSDv)</f>
-        <v>2.2505720822583455</v>
+        <v>6.7517239593760845</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
       </c>
       <c r="F26">
         <f>(TAN(0.5*IRFOV*PI()/180)-TAN(-0.5*IRFOV*PI()/180))*OperatingAltitude/3.281</f>
-        <v>252.49226600005792</v>
+        <v>609.5702529716549</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
       </c>
       <c r="F27">
         <f>IR_GroundSwath*CruisingVelocity*1.852/3.6</f>
-        <v>12989.324350891871</v>
+        <v>31359.00301398625</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -815,14 +815,14 @@
       </c>
       <c r="F29">
         <f>I29/I30</f>
-        <v>0.11940624924274684</v>
+        <v>0.84483891340375505</v>
       </c>
       <c r="H29" t="s">
         <v>19</v>
       </c>
       <c r="I29">
         <f>(IR_N_Human/0.75)^(2.7+0.7*(IR_N_Human/C4))</f>
-        <v>0.13559742973427333</v>
+        <v>5.4449149070615048</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -831,7 +831,7 @@
       </c>
       <c r="I30">
         <f>1+I29</f>
-        <v>1.1355974297342732</v>
+        <v>6.4449149070615048</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -840,14 +840,14 @@
       </c>
       <c r="F31">
         <f>I31/I32</f>
-        <v>0.99490884300249272</v>
+        <v>0.99999999743384027</v>
       </c>
       <c r="H31" t="s">
         <v>19</v>
       </c>
       <c r="I31">
         <f>(IR_N_Vehicle/0.75)^(2.7+0.7*(IR_N_Vehicle/C4))</f>
-        <v>195.41900662062224</v>
+        <v>389687355.66656601</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
       </c>
       <c r="I32">
         <f>1+I31</f>
-        <v>196.41900662062224</v>
+        <v>389687356.66656601</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
@@ -864,8 +864,8 @@
         <v>35</v>
       </c>
       <c r="F33">
-        <f>25000000*60/IR_Ground_Coverage_Rate</f>
-        <v>115479.44754316703</v>
+        <f>25000*60/IR_Ground_Coverage_Rate</f>
+        <v>47.833153347732186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>